<commit_message>
Working on model & analysis.py for pm2_batch
-to compare RMSE
</commit_message>
<xml_diff>
--- a/exposan/pm2_batch/data/batch_exp_result.xlsx
+++ b/exposan/pm2_batch/data/batch_exp_result.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Downloads\EXPOsan\exposan\pm2_batch\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{19BF9313-83DA-452E-857A-6AA38EDBF604}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F970EFB-ED55-417F-AC10-A396CBC28FC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{EC7A2F61-3DDC-4A57-B61E-94C79A6F2846}"/>
   </bookViews>
@@ -25,11 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="4">
-  <si>
-    <t>Time (day)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>VSS</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -40,6 +36,10 @@
   </si>
   <si>
     <t>S_P</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>t_stamp</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -422,7 +422,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -432,16 +432,16 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>